<commit_message>
adding farm and breed type to excel import
</commit_message>
<xml_diff>
--- a/eg.xlsx
+++ b/eg.xlsx
@@ -77,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -98,12 +98,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -168,7 +162,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,15 +175,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -198,10 +188,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,7 +275,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,9 +285,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="7.18"/>
   </cols>
@@ -315,54 +301,54 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="1"/>
@@ -372,119 +358,119 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7" t="n">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="7" t="n">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="0"/>
-      <c r="O10" s="0"/>
-      <c r="P10" s="0"/>
-      <c r="Q10" s="0"/>
-      <c r="R10" s="0"/>
-      <c r="S10" s="0"/>
-      <c r="T10" s="0"/>
-      <c r="U10" s="0"/>
-      <c r="V10" s="0"/>
-      <c r="W10" s="0"/>
-      <c r="X10" s="0"/>
-      <c r="Y10" s="0"/>
-      <c r="Z10" s="0"/>
-      <c r="AA10" s="0"/>
-      <c r="AB10" s="0"/>
-      <c r="AC10" s="0"/>
-      <c r="AD10" s="0"/>
-      <c r="AE10" s="0"/>
-      <c r="AF10" s="0"/>
-      <c r="AG10" s="0"/>
-      <c r="AH10" s="0"/>
-      <c r="AI10" s="0"/>
-      <c r="AJ10" s="0"/>
-      <c r="AK10" s="0"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="9"/>
+      <c r="J11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
active and flock field to chicken form
</commit_message>
<xml_diff>
--- a/eg.xlsx
+++ b/eg.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Batch</t>
   </si>
   <si>
-    <t xml:space="preserve">Days Alive</t>
+    <t xml:space="preserve">Mortality</t>
   </si>
   <si>
     <t xml:space="preserve">Weight</t>
@@ -275,7 +275,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chicken detail form excel
</commit_message>
<xml_diff>
--- a/eg.xlsx
+++ b/eg.xlsx
@@ -275,7 +275,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,7 +367,9 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="n">
+        <v>601</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>

</xml_diff>

<commit_message>
stirngify chicken import errors
</commit_message>
<xml_diff>
--- a/eg.xlsx
+++ b/eg.xlsx
@@ -74,8 +74,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -162,7 +163,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +185,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,7 +280,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -366,23 +371,25 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="6" t="n">
+        <v>44573</v>
+      </c>
       <c r="F3" s="5" t="n">
         <v>601</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6" t="n">
+      <c r="J3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -398,16 +405,16 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6" t="n">
+      <c r="J4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -423,20 +430,20 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -476,7 +483,7 @@
       <c r="AK10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="7"/>
+      <c r="J11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fixing dead date view
</commit_message>
<xml_diff>
--- a/eg.xlsx
+++ b/eg.xlsx
@@ -280,7 +280,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -402,7 +402,9 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="7" t="n">
@@ -427,7 +429,9 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="5" t="n">
+        <v>2</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="7" t="n">

</xml_diff>

<commit_message>
fix feed, egg and weight create from excel
</commit_message>
<xml_diff>
--- a/eg.xlsx
+++ b/eg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
@@ -280,10 +280,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK11"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
+      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,7 +409,7 @@
       <c r="M3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -439,47 +439,39 @@
       <c r="M4" s="7" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>10</v>
-      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="8"/>
     </row>
     <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
@@ -487,7 +479,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="0"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -495,33 +487,30 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="8"/>
+      <c r="N10" s="0"/>
+      <c r="O10" s="0"/>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
+      <c r="S10" s="0"/>
+      <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="Z10" s="0"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="0"/>
+      <c r="AC10" s="0"/>
+      <c r="AD10" s="0"/>
+      <c r="AE10" s="0"/>
+      <c r="AF10" s="0"/>
+      <c r="AG10" s="0"/>
+      <c r="AH10" s="0"/>
+      <c r="AI10" s="0"/>
+      <c r="AJ10" s="0"/>
+      <c r="AK10" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>